<commit_message>
updated script and data folder
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\PycharmProjects\pythonProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\PycharmProjects\fhir_questionnaire_item_populator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAA5AFA-05F5-42AA-96DF-846E3EE6DC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A0B431-274D-4EAE-8F4C-82C0B69810CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6CCBEFA-14F7-4D58-B784-0C5A9DA8EF6F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D6CCBEFA-14F7-4D58-B784-0C5A9DA8EF6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>linkid</t>
   </si>
@@ -127,22 +127,51 @@
   </si>
   <si>
     <t>J’ai été vu·e dès que cela m’a semblé nécessaire</t>
+  </si>
+  <si>
+    <t>Wurden bei Ihnen in den letzten 12 Monate eine oder mehrere diagnostische Untersuchungen wegen Krebs in dem im Einladungsschreiben genannten Spital durchgeführt, wie zum Beispiel eine Endoskopie, eine Biopsie, eine Mammographie oder eine Computertomographie?</t>
+  </si>
+  <si>
+    <t>Au cours des 12 derniers mois, avez-vous effectué un ou plusieurs examens diagnostiques pour le cancer, tels qu’une endoscopie, une biopsie, une mammographie ou un scanner, à l’hôpital mentionné dans la lettre d’invitation ?</t>
+  </si>
+  <si>
+    <t>Avant l’examen, aviez-vous toutes les informations dont vous aviez besoin concernant cet examen ?</t>
+  </si>
+  <si>
+    <t>Haben Sie vor der Untersuchung alle Informationen erhalten, die Sie darüber benötigten?</t>
+  </si>
+  <si>
+    <t>Ja, absolut</t>
+  </si>
+  <si>
+    <t>Ja, bis zu einem gewissen Grad</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>Oui, tout à fait</t>
+  </si>
+  <si>
+    <t>Oui, dans une certaine mesure</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Oui</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -168,12 +197,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -189,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -505,30 +533,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940D8FA8-F46D-42CA-8551-324811725356}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="58.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="142.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="66.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="150.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -657,17 +675,75 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:18" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E7" s="1"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -682,7 +758,7 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>